<commit_message>
update raw data file
</commit_message>
<xml_diff>
--- a/LGD_2006/20210203_LGD-2006_RawTypingFile.xlsx
+++ b/LGD_2006/20210203_LGD-2006_RawTypingFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tumha\Desktop\Lab Work\Data\Sorting data\LGD_2006\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tumha\Desktop\Lab Work\Sorting data\sorting_data_curate\LGD_2006\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80BB23A-F412-400C-A29F-E9A2C8BB77D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41168C0E-345A-4EBD-93A7-099E01F09CF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{B206CDC5-95C4-4D0D-947C-04486EE88E18}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Polychaeta" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Size!$A$1:$R$1117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Size!$A$1:$R$1119</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4910" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4931" uniqueCount="107">
   <si>
     <t>Cruise</t>
   </si>
@@ -752,8 +752,8 @@
   <dimension ref="A1:R1119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1000" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1119" sqref="N1119"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q379" sqref="Q379:Q1119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -988,7 +988,7 @@
         <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L8">
         <v>100</v>
@@ -1016,7 +1016,7 @@
         <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L9">
         <v>100</v>
@@ -1044,7 +1044,7 @@
         <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L10">
         <v>90</v>
@@ -1072,7 +1072,7 @@
         <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L11">
         <v>40</v>
@@ -1100,7 +1100,7 @@
         <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L12">
         <v>90</v>
@@ -1128,7 +1128,7 @@
         <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L13">
         <v>70</v>
@@ -1156,7 +1156,7 @@
         <v>26</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L14">
         <v>30</v>
@@ -1767,7 +1767,7 @@
         <v>26</v>
       </c>
       <c r="J39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L39">
         <v>150</v>
@@ -1793,7 +1793,7 @@
         <v>26</v>
       </c>
       <c r="J40" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L40">
         <v>40</v>
@@ -1819,7 +1819,7 @@
         <v>26</v>
       </c>
       <c r="J41" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L41">
         <v>20</v>
@@ -1845,7 +1845,7 @@
         <v>26</v>
       </c>
       <c r="J42" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L42">
         <v>50</v>
@@ -1871,7 +1871,7 @@
         <v>26</v>
       </c>
       <c r="J43" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L43">
         <v>23</v>
@@ -1897,7 +1897,7 @@
         <v>26</v>
       </c>
       <c r="J44" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L44">
         <v>40</v>
@@ -2899,7 +2899,7 @@
         <v>26</v>
       </c>
       <c r="J86" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L86">
         <v>30</v>
@@ -2925,7 +2925,7 @@
         <v>26</v>
       </c>
       <c r="J87" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L87">
         <v>90</v>
@@ -2951,7 +2951,7 @@
         <v>26</v>
       </c>
       <c r="J88" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L88">
         <v>54</v>
@@ -2977,7 +2977,7 @@
         <v>26</v>
       </c>
       <c r="J89" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L89">
         <v>150</v>
@@ -3003,7 +3003,7 @@
         <v>26</v>
       </c>
       <c r="J90" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L90">
         <v>100</v>
@@ -3029,7 +3029,7 @@
         <v>26</v>
       </c>
       <c r="J91" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L91">
         <v>70</v>
@@ -3055,7 +3055,7 @@
         <v>26</v>
       </c>
       <c r="J92" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L92">
         <v>30</v>
@@ -3357,7 +3357,7 @@
         <v>26</v>
       </c>
       <c r="J105" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L105">
         <v>50</v>
@@ -3383,7 +3383,7 @@
         <v>26</v>
       </c>
       <c r="J106" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L106">
         <v>24</v>
@@ -3409,7 +3409,7 @@
         <v>26</v>
       </c>
       <c r="J107" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L107">
         <v>95</v>
@@ -3435,7 +3435,7 @@
         <v>26</v>
       </c>
       <c r="J108" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L108">
         <v>70</v>
@@ -3447,7 +3447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:17" hidden="1">
+    <row r="109" spans="1:17">
       <c r="A109" s="3" t="s">
         <v>17</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>42</v>
       </c>
       <c r="J109" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L109">
         <v>90</v>
@@ -4403,7 +4403,7 @@
         <v>26</v>
       </c>
       <c r="J148" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L148">
         <v>42</v>
@@ -8242,7 +8242,7 @@
         <v>26</v>
       </c>
       <c r="J311" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L311">
         <v>2.5</v>
@@ -9625,7 +9625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="369" spans="1:13" hidden="1">
+    <row r="369" spans="1:17" hidden="1">
       <c r="A369" s="3" t="s">
         <v>17</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="370" spans="1:13" hidden="1">
+    <row r="370" spans="1:17" hidden="1">
       <c r="A370" s="3" t="s">
         <v>17</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="371" spans="1:13" hidden="1">
+    <row r="371" spans="1:17" hidden="1">
       <c r="A371" s="3" t="s">
         <v>17</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="372" spans="1:13" hidden="1">
+    <row r="372" spans="1:17" hidden="1">
       <c r="A372" s="3" t="s">
         <v>17</v>
       </c>
@@ -9717,7 +9717,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="373" spans="1:13" hidden="1">
+    <row r="373" spans="1:17" hidden="1">
       <c r="A373" s="3" t="s">
         <v>17</v>
       </c>
@@ -9740,7 +9740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:13" hidden="1">
+    <row r="374" spans="1:17" hidden="1">
       <c r="A374" s="3" t="s">
         <v>17</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="375" spans="1:13" hidden="1">
+    <row r="375" spans="1:17" hidden="1">
       <c r="A375" s="3" t="s">
         <v>17</v>
       </c>
@@ -9786,7 +9786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:13" hidden="1">
+    <row r="376" spans="1:17" hidden="1">
       <c r="A376" s="3" t="s">
         <v>17</v>
       </c>
@@ -9809,7 +9809,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="377" spans="1:13" hidden="1">
+    <row r="377" spans="1:17" hidden="1">
       <c r="A377" s="3" t="s">
         <v>17</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="378" spans="1:13" hidden="1">
+    <row r="378" spans="1:17" hidden="1">
       <c r="A378" s="3" t="s">
         <v>17</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="379" spans="1:13" hidden="1">
+    <row r="379" spans="1:17">
       <c r="A379" s="3" t="s">
         <v>17</v>
       </c>
@@ -9877,8 +9877,11 @@
       <c r="M379">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="380" spans="1:13" hidden="1">
+      <c r="Q379" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="380" spans="1:17">
       <c r="A380" s="3" t="s">
         <v>17</v>
       </c>
@@ -9900,8 +9903,11 @@
       <c r="M380">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="381" spans="1:13" hidden="1">
+      <c r="Q380" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="381" spans="1:17">
       <c r="A381" s="3" t="s">
         <v>17</v>
       </c>
@@ -9923,8 +9929,11 @@
       <c r="M381">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="382" spans="1:13" hidden="1">
+      <c r="Q381" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="382" spans="1:17">
       <c r="A382" s="3" t="s">
         <v>17</v>
       </c>
@@ -9946,8 +9955,11 @@
       <c r="M382">
         <v>1</v>
       </c>
-    </row>
-    <row r="383" spans="1:13" hidden="1">
+      <c r="Q382" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="383" spans="1:17">
       <c r="A383" s="3" t="s">
         <v>17</v>
       </c>
@@ -9969,8 +9981,11 @@
       <c r="M383">
         <v>1</v>
       </c>
-    </row>
-    <row r="384" spans="1:13" hidden="1">
+      <c r="Q383" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="384" spans="1:17">
       <c r="A384" s="3" t="s">
         <v>17</v>
       </c>
@@ -9992,8 +10007,11 @@
       <c r="M384">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="385" spans="1:13" hidden="1">
+      <c r="Q384" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="385" spans="1:17">
       <c r="A385" s="3" t="s">
         <v>17</v>
       </c>
@@ -10015,8 +10033,11 @@
       <c r="M385">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="386" spans="1:13" hidden="1">
+      <c r="Q385" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="386" spans="1:17">
       <c r="A386" s="3" t="s">
         <v>17</v>
       </c>
@@ -10038,8 +10059,11 @@
       <c r="M386">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="387" spans="1:13" hidden="1">
+      <c r="Q386" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="387" spans="1:17">
       <c r="A387" s="3" t="s">
         <v>17</v>
       </c>
@@ -10061,8 +10085,11 @@
       <c r="M387">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="388" spans="1:13" hidden="1">
+      <c r="Q387" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="388" spans="1:17">
       <c r="A388" s="3" t="s">
         <v>17</v>
       </c>
@@ -10084,8 +10111,11 @@
       <c r="M388">
         <v>1</v>
       </c>
-    </row>
-    <row r="389" spans="1:13" hidden="1">
+      <c r="Q388" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="389" spans="1:17">
       <c r="A389" s="3" t="s">
         <v>17</v>
       </c>
@@ -10107,8 +10137,11 @@
       <c r="M389">
         <v>1</v>
       </c>
-    </row>
-    <row r="390" spans="1:13" hidden="1">
+      <c r="Q389" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="390" spans="1:17">
       <c r="A390" s="3" t="s">
         <v>17</v>
       </c>
@@ -10130,8 +10163,11 @@
       <c r="M390">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="391" spans="1:13" hidden="1">
+      <c r="Q390" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="391" spans="1:17">
       <c r="A391" s="3" t="s">
         <v>17</v>
       </c>
@@ -10153,8 +10189,11 @@
       <c r="M391">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="392" spans="1:13" hidden="1">
+      <c r="Q391" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="392" spans="1:17">
       <c r="A392" s="3" t="s">
         <v>17</v>
       </c>
@@ -10176,8 +10215,11 @@
       <c r="M392">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="393" spans="1:13" hidden="1">
+      <c r="Q392" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="393" spans="1:17">
       <c r="A393" s="3" t="s">
         <v>17</v>
       </c>
@@ -10199,8 +10241,11 @@
       <c r="M393">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="394" spans="1:13" hidden="1">
+      <c r="Q393" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="394" spans="1:17">
       <c r="A394" s="3" t="s">
         <v>17</v>
       </c>
@@ -10222,8 +10267,11 @@
       <c r="M394">
         <v>1</v>
       </c>
-    </row>
-    <row r="395" spans="1:13" hidden="1">
+      <c r="Q394" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="395" spans="1:17">
       <c r="A395" s="3" t="s">
         <v>17</v>
       </c>
@@ -10245,8 +10293,11 @@
       <c r="M395">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="396" spans="1:13" hidden="1">
+      <c r="Q395" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="396" spans="1:17">
       <c r="A396" s="3" t="s">
         <v>17</v>
       </c>
@@ -10268,8 +10319,11 @@
       <c r="M396">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="397" spans="1:13" hidden="1">
+      <c r="Q396" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="397" spans="1:17">
       <c r="A397" s="3" t="s">
         <v>17</v>
       </c>
@@ -10291,8 +10345,11 @@
       <c r="M397">
         <v>1</v>
       </c>
-    </row>
-    <row r="398" spans="1:13" hidden="1">
+      <c r="Q397" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="398" spans="1:17">
       <c r="A398" s="3" t="s">
         <v>17</v>
       </c>
@@ -10314,8 +10371,11 @@
       <c r="M398">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="399" spans="1:13" hidden="1">
+      <c r="Q398" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="399" spans="1:17">
       <c r="A399" s="3" t="s">
         <v>17</v>
       </c>
@@ -10337,8 +10397,11 @@
       <c r="M399">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="400" spans="1:13" hidden="1">
+      <c r="Q399" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="400" spans="1:17" hidden="1">
       <c r="A400" s="3" t="s">
         <v>17</v>
       </c>
@@ -11161,7 +11224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="435" spans="1:17" hidden="1">
+    <row r="435" spans="1:17">
       <c r="A435" s="3" t="s">
         <v>17</v>
       </c>
@@ -11175,7 +11238,7 @@
         <v>42</v>
       </c>
       <c r="J435" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L435">
         <v>17</v>
@@ -11187,7 +11250,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="436" spans="1:17" hidden="1">
+    <row r="436" spans="1:17">
       <c r="A436" s="3" t="s">
         <v>17</v>
       </c>
@@ -11201,7 +11264,7 @@
         <v>42</v>
       </c>
       <c r="J436" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L436">
         <v>25</v>
@@ -11213,7 +11276,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="437" spans="1:17" hidden="1">
+    <row r="437" spans="1:17">
       <c r="A437" s="3" t="s">
         <v>17</v>
       </c>
@@ -11227,7 +11290,7 @@
         <v>42</v>
       </c>
       <c r="J437" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L437">
         <v>7</v>
@@ -11239,7 +11302,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="438" spans="1:17" hidden="1">
+    <row r="438" spans="1:17">
       <c r="A438" s="3" t="s">
         <v>17</v>
       </c>
@@ -11253,7 +11316,7 @@
         <v>42</v>
       </c>
       <c r="J438" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L438">
         <v>35</v>
@@ -11265,7 +11328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="439" spans="1:17" hidden="1">
+    <row r="439" spans="1:17">
       <c r="A439" s="3" t="s">
         <v>17</v>
       </c>
@@ -11279,7 +11342,7 @@
         <v>42</v>
       </c>
       <c r="J439" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L439">
         <v>10</v>
@@ -11512,7 +11575,7 @@
         <v>26</v>
       </c>
       <c r="J449" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L449">
         <v>4</v>
@@ -12943,7 +13006,7 @@
         <v>26</v>
       </c>
       <c r="J509" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L509">
         <v>2.5</v>
@@ -12969,7 +13032,7 @@
         <v>26</v>
       </c>
       <c r="J510" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L510">
         <v>3</v>
@@ -13941,7 +14004,7 @@
         <v>26</v>
       </c>
       <c r="J552" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L552">
         <v>3</v>
@@ -14059,7 +14122,7 @@
         <v>26</v>
       </c>
       <c r="J557" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L557">
         <v>5</v>
@@ -14085,7 +14148,7 @@
         <v>26</v>
       </c>
       <c r="J558" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L558">
         <v>5</v>
@@ -14111,7 +14174,7 @@
         <v>26</v>
       </c>
       <c r="J559" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L559">
         <v>7.5</v>
@@ -14137,7 +14200,7 @@
         <v>26</v>
       </c>
       <c r="J560" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L560">
         <v>8</v>
@@ -14163,7 +14226,7 @@
         <v>26</v>
       </c>
       <c r="J561" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L561">
         <v>4</v>
@@ -14189,7 +14252,7 @@
         <v>26</v>
       </c>
       <c r="J562" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L562">
         <v>30</v>
@@ -14215,7 +14278,7 @@
         <v>26</v>
       </c>
       <c r="J563" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L563">
         <v>3</v>
@@ -14241,7 +14304,7 @@
         <v>26</v>
       </c>
       <c r="J564" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L564">
         <v>2</v>
@@ -14267,7 +14330,7 @@
         <v>26</v>
       </c>
       <c r="J565" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L565">
         <v>3</v>
@@ -14293,7 +14356,7 @@
         <v>26</v>
       </c>
       <c r="J566" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L566">
         <v>2</v>
@@ -14319,7 +14382,7 @@
         <v>26</v>
       </c>
       <c r="J567" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L567">
         <v>3</v>
@@ -14789,7 +14852,7 @@
         <v>26</v>
       </c>
       <c r="J586" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L586">
         <v>1.5</v>
@@ -15081,7 +15144,7 @@
         <v>26</v>
       </c>
       <c r="J597" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L597">
         <v>15</v>
@@ -15107,7 +15170,7 @@
         <v>26</v>
       </c>
       <c r="J598" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L598">
         <v>8</v>
@@ -15133,7 +15196,7 @@
         <v>26</v>
       </c>
       <c r="J599" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L599">
         <v>12</v>
@@ -15159,7 +15222,7 @@
         <v>26</v>
       </c>
       <c r="J600" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L600">
         <v>9</v>
@@ -15185,7 +15248,7 @@
         <v>26</v>
       </c>
       <c r="J601" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L601">
         <v>7</v>
@@ -15211,7 +15274,7 @@
         <v>26</v>
       </c>
       <c r="J602" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L602">
         <v>9</v>
@@ -15237,7 +15300,7 @@
         <v>26</v>
       </c>
       <c r="J603" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L603">
         <v>12</v>
@@ -15263,7 +15326,7 @@
         <v>26</v>
       </c>
       <c r="J604" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L604">
         <v>7</v>
@@ -15289,7 +15352,7 @@
         <v>26</v>
       </c>
       <c r="J605" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L605">
         <v>4</v>
@@ -15315,7 +15378,7 @@
         <v>26</v>
       </c>
       <c r="J606" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L606">
         <v>9</v>
@@ -15341,7 +15404,7 @@
         <v>26</v>
       </c>
       <c r="J607" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L607">
         <v>6</v>
@@ -15367,7 +15430,7 @@
         <v>26</v>
       </c>
       <c r="J608" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L608">
         <v>7</v>
@@ -15393,7 +15456,7 @@
         <v>26</v>
       </c>
       <c r="J609" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L609">
         <v>10</v>
@@ -15419,7 +15482,7 @@
         <v>26</v>
       </c>
       <c r="J610" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L610">
         <v>6</v>
@@ -15445,7 +15508,7 @@
         <v>26</v>
       </c>
       <c r="J611" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L611">
         <v>7</v>
@@ -15471,7 +15534,7 @@
         <v>26</v>
       </c>
       <c r="J612" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L612">
         <v>5</v>
@@ -15497,7 +15560,7 @@
         <v>26</v>
       </c>
       <c r="J613" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L613">
         <v>11</v>
@@ -15523,7 +15586,7 @@
         <v>26</v>
       </c>
       <c r="J614" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L614">
         <v>3</v>
@@ -15549,7 +15612,7 @@
         <v>26</v>
       </c>
       <c r="J615" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L615">
         <v>10</v>
@@ -15575,7 +15638,7 @@
         <v>26</v>
       </c>
       <c r="J616" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L616">
         <v>10</v>
@@ -15601,7 +15664,7 @@
         <v>26</v>
       </c>
       <c r="J617" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L617">
         <v>10</v>
@@ -15627,7 +15690,7 @@
         <v>26</v>
       </c>
       <c r="J618" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L618">
         <v>6</v>
@@ -15653,7 +15716,7 @@
         <v>26</v>
       </c>
       <c r="J619" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L619">
         <v>14</v>
@@ -16665,7 +16728,7 @@
         <v>26</v>
       </c>
       <c r="J660" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L660">
         <v>4</v>
@@ -16691,7 +16754,7 @@
         <v>26</v>
       </c>
       <c r="J661" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L661">
         <v>5</v>
@@ -16717,7 +16780,7 @@
         <v>26</v>
       </c>
       <c r="J662" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L662">
         <v>5</v>
@@ -17261,7 +17324,7 @@
         <v>26</v>
       </c>
       <c r="J685" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L685">
         <v>3.5</v>
@@ -17287,7 +17350,7 @@
         <v>26</v>
       </c>
       <c r="J686" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L686">
         <v>5</v>
@@ -17313,7 +17376,7 @@
         <v>26</v>
       </c>
       <c r="J687" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L687">
         <v>3.75</v>
@@ -17339,7 +17402,7 @@
         <v>26</v>
       </c>
       <c r="J688" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L688">
         <v>5</v>
@@ -19644,7 +19707,7 @@
         <v>26</v>
       </c>
       <c r="J783" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L783">
         <v>5</v>
@@ -20254,7 +20317,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="810" spans="1:17" hidden="1">
+    <row r="810" spans="1:17">
       <c r="A810" s="3" t="s">
         <v>17</v>
       </c>
@@ -20268,7 +20331,7 @@
         <v>42</v>
       </c>
       <c r="J810" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L810">
         <v>7.5</v>
@@ -20294,7 +20357,7 @@
         <v>26</v>
       </c>
       <c r="J811" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L811">
         <v>3.5</v>
@@ -20320,7 +20383,7 @@
         <v>26</v>
       </c>
       <c r="J812" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L812">
         <v>5</v>
@@ -20346,7 +20409,7 @@
         <v>26</v>
       </c>
       <c r="J813" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L813">
         <v>7</v>
@@ -20372,7 +20435,7 @@
         <v>26</v>
       </c>
       <c r="J814" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L814">
         <v>4</v>
@@ -20398,7 +20461,7 @@
         <v>26</v>
       </c>
       <c r="J815" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L815">
         <v>4</v>
@@ -20424,7 +20487,7 @@
         <v>26</v>
       </c>
       <c r="J816" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L816">
         <v>2</v>
@@ -20450,7 +20513,7 @@
         <v>26</v>
       </c>
       <c r="J817" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L817">
         <v>5</v>
@@ -20476,7 +20539,7 @@
         <v>26</v>
       </c>
       <c r="J818" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L818">
         <v>3</v>
@@ -20502,7 +20565,7 @@
         <v>26</v>
       </c>
       <c r="J819" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L819">
         <v>5</v>
@@ -20528,7 +20591,7 @@
         <v>26</v>
       </c>
       <c r="J820" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L820">
         <v>2</v>
@@ -20554,7 +20617,7 @@
         <v>26</v>
       </c>
       <c r="J821" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L821">
         <v>2</v>
@@ -20580,7 +20643,7 @@
         <v>26</v>
       </c>
       <c r="J822" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L822">
         <v>2</v>
@@ -20606,7 +20669,7 @@
         <v>26</v>
       </c>
       <c r="J823" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L823">
         <v>2.5</v>
@@ -20632,7 +20695,7 @@
         <v>26</v>
       </c>
       <c r="J824" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L824">
         <v>3.5</v>
@@ -20658,7 +20721,7 @@
         <v>26</v>
       </c>
       <c r="J825" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L825">
         <v>2.5</v>
@@ -20684,7 +20747,7 @@
         <v>26</v>
       </c>
       <c r="J826" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L826">
         <v>3.75</v>
@@ -20710,7 +20773,7 @@
         <v>26</v>
       </c>
       <c r="J827" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L827">
         <v>2.5</v>
@@ -20736,7 +20799,7 @@
         <v>26</v>
       </c>
       <c r="J828" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L828">
         <v>2</v>
@@ -20762,7 +20825,7 @@
         <v>26</v>
       </c>
       <c r="J829" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L829">
         <v>3</v>
@@ -23232,7 +23295,7 @@
         <v>26</v>
       </c>
       <c r="J936" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L936">
         <v>4</v>
@@ -23258,7 +23321,7 @@
         <v>26</v>
       </c>
       <c r="J937" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L937">
         <v>3</v>
@@ -23284,7 +23347,7 @@
         <v>26</v>
       </c>
       <c r="J938" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L938">
         <v>3</v>
@@ -23310,7 +23373,7 @@
         <v>26</v>
       </c>
       <c r="J939" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L939">
         <v>3.5</v>
@@ -23336,7 +23399,7 @@
         <v>26</v>
       </c>
       <c r="J940" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L940">
         <v>3</v>
@@ -24452,7 +24515,7 @@
         <v>26</v>
       </c>
       <c r="J988" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L988">
         <v>2.5</v>
@@ -24478,7 +24541,7 @@
         <v>26</v>
       </c>
       <c r="J989" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L989">
         <v>4</v>
@@ -24504,7 +24567,7 @@
         <v>26</v>
       </c>
       <c r="J990" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L990">
         <v>5</v>
@@ -24530,7 +24593,7 @@
         <v>26</v>
       </c>
       <c r="J991" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L991">
         <v>5</v>
@@ -24556,7 +24619,7 @@
         <v>26</v>
       </c>
       <c r="J992" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L992">
         <v>4</v>
@@ -24582,7 +24645,7 @@
         <v>26</v>
       </c>
       <c r="J993" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L993">
         <v>4</v>
@@ -24608,7 +24671,7 @@
         <v>26</v>
       </c>
       <c r="J994" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L994">
         <v>6.5</v>
@@ -24634,7 +24697,7 @@
         <v>26</v>
       </c>
       <c r="J995" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L995">
         <v>5</v>
@@ -24660,7 +24723,7 @@
         <v>26</v>
       </c>
       <c r="J996" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L996">
         <v>9</v>
@@ -24686,7 +24749,7 @@
         <v>26</v>
       </c>
       <c r="J997" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L997">
         <v>5</v>
@@ -24712,7 +24775,7 @@
         <v>26</v>
       </c>
       <c r="J998" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L998">
         <v>3</v>
@@ -24738,7 +24801,7 @@
         <v>26</v>
       </c>
       <c r="J999" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L999">
         <v>6</v>
@@ -24764,7 +24827,7 @@
         <v>26</v>
       </c>
       <c r="J1000" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1000">
         <v>0.5</v>
@@ -24790,7 +24853,7 @@
         <v>26</v>
       </c>
       <c r="J1001" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1001">
         <v>5</v>
@@ -24816,7 +24879,7 @@
         <v>26</v>
       </c>
       <c r="J1002" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1002">
         <v>2</v>
@@ -24842,7 +24905,7 @@
         <v>26</v>
       </c>
       <c r="J1003" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1003">
         <v>1</v>
@@ -24868,7 +24931,7 @@
         <v>26</v>
       </c>
       <c r="J1004" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1004">
         <v>2</v>
@@ -24894,7 +24957,7 @@
         <v>26</v>
       </c>
       <c r="J1005" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1005">
         <v>2</v>
@@ -24920,7 +24983,7 @@
         <v>26</v>
       </c>
       <c r="J1006" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1006">
         <v>35</v>
@@ -27368,7 +27431,7 @@
         <v>26</v>
       </c>
       <c r="J1111" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1111">
         <v>1.5</v>
@@ -27394,7 +27457,7 @@
         <v>26</v>
       </c>
       <c r="J1112" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1112">
         <v>2.5</v>
@@ -27420,7 +27483,7 @@
         <v>26</v>
       </c>
       <c r="J1113" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1113">
         <v>2.5</v>
@@ -27446,7 +27509,7 @@
         <v>26</v>
       </c>
       <c r="J1114" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1114">
         <v>1.5</v>
@@ -27472,7 +27535,7 @@
         <v>26</v>
       </c>
       <c r="J1115" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L1115">
         <v>1.5</v>
@@ -27530,7 +27593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1118" spans="1:17">
+    <row r="1118" spans="1:17" hidden="1">
       <c r="A1118" t="s">
         <v>17</v>
       </c>
@@ -27553,7 +27616,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="1119" spans="1:17">
+    <row r="1119" spans="1:17" hidden="1">
       <c r="A1119" t="s">
         <v>17</v>
       </c>
@@ -27577,9 +27640,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1117" xr:uid="{637DB578-4D2D-4B05-A810-D199B4D586E4}">
+  <autoFilter ref="A1:R1119" xr:uid="{637DB578-4D2D-4B05-A810-D199B4D586E4}">
     <filterColumn colId="6">
       <filters>
+        <filter val="Bryozoa"/>
+        <filter val="Entoprocta"/>
         <filter val="Hydrozoa"/>
       </filters>
     </filterColumn>

</xml_diff>